<commit_message>
added a debug command for the microbit
</commit_message>
<xml_diff>
--- a/SN8 i2c & pins.xlsx
+++ b/SN8 i2c & pins.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\targetarchitecture\esp32-rainbow-sparkle-unicorn\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{353C1DEC-7CDB-42C1-B0CB-D2E9C7FC1F36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8DFAD64-7952-4D5B-B523-340525B5FDF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13872" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="685" uniqueCount="392">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="688" uniqueCount="394">
   <si>
     <t>Action</t>
   </si>
@@ -1220,6 +1220,12 @@
   <si>
     <t>TSTATE</t>
   </si>
+  <si>
+    <t>DEBUG</t>
+  </si>
+  <si>
+    <t>message</t>
+  </si>
 </sst>
 </file>
 
@@ -30075,10 +30081,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{784B3CAF-F768-478D-8F53-9C6BB6D54AC2}">
-  <dimension ref="A1:G47"/>
+  <dimension ref="A1:G48"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+      <selection activeCell="D48" sqref="D48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.45"/>
@@ -30896,6 +30902,17 @@
         <v>387</v>
       </c>
       <c r="C47" s="57"/>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A48" s="33" t="s">
+        <v>343</v>
+      </c>
+      <c r="B48" s="57" t="s">
+        <v>392</v>
+      </c>
+      <c r="D48" s="43" t="s">
+        <v>393</v>
+      </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:G45" xr:uid="{784B3CAF-F768-478D-8F53-9C6BB6D54AC2}">

</xml_diff>

<commit_message>
wifi manager not working well
</commit_message>
<xml_diff>
--- a/SN8 i2c & pins.xlsx
+++ b/SN8 i2c & pins.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\targetarchitecture\esp32-rainbow-sparkle-unicorn\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8DFAD64-7952-4D5B-B523-340525B5FDF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{004D3D64-5373-4708-A738-5C7B1163CA58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13872" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="688" uniqueCount="394">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="697" uniqueCount="397">
   <si>
     <t>Action</t>
   </si>
@@ -1203,12 +1203,6 @@
     <t>From ESP32</t>
   </si>
   <si>
-    <t>Starting</t>
-  </si>
-  <si>
-    <t>STARTING</t>
-  </si>
-  <si>
     <t>TUPDATE</t>
   </si>
   <si>
@@ -1225,6 +1219,21 @@
   </si>
   <si>
     <t>message</t>
+  </si>
+  <si>
+    <t>topic , message</t>
+  </si>
+  <si>
+    <t>PUBLISH</t>
+  </si>
+  <si>
+    <t>SUBSCRIBE</t>
+  </si>
+  <si>
+    <t>UNSUBSCRIBE</t>
+  </si>
+  <si>
+    <t>IoT</t>
   </si>
 </sst>
 </file>
@@ -30081,10 +30090,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{784B3CAF-F768-478D-8F53-9C6BB6D54AC2}">
-  <dimension ref="A1:G48"/>
+  <dimension ref="A1:G51"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D48" sqref="D48"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A51" sqref="A51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.45"/>
@@ -30604,10 +30613,10 @@
         <v>98</v>
       </c>
       <c r="B28" s="57" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="C28" s="57" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="D28" s="48"/>
       <c r="E28" s="68"/>
@@ -30624,7 +30633,7 @@
       </c>
       <c r="B29" s="57"/>
       <c r="C29" s="57" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="D29" s="48"/>
       <c r="E29" s="68"/>
@@ -30863,10 +30872,10 @@
         <v>87</v>
       </c>
       <c r="B45" s="43" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="C45" s="43" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="D45" s="53"/>
       <c r="E45" s="53"/>
@@ -30883,7 +30892,7 @@
       </c>
       <c r="B46" s="57"/>
       <c r="C46" s="57" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="D46" s="53"/>
       <c r="E46" s="53"/>
@@ -30896,22 +30905,54 @@
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A47" s="33" t="s">
-        <v>386</v>
+        <v>343</v>
       </c>
       <c r="B47" s="57" t="s">
-        <v>387</v>
-      </c>
-      <c r="C47" s="57"/>
+        <v>390</v>
+      </c>
+      <c r="D47" s="43" t="s">
+        <v>391</v>
+      </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A48" s="33" t="s">
-        <v>343</v>
-      </c>
-      <c r="B48" s="57" t="s">
+        <v>396</v>
+      </c>
+      <c r="C48" s="43" t="s">
+        <v>323</v>
+      </c>
+      <c r="D48" s="43" t="s">
         <v>392</v>
       </c>
-      <c r="D48" s="43" t="s">
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A49" s="33" t="s">
+        <v>396</v>
+      </c>
+      <c r="B49" s="57" t="s">
         <v>393</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A50" s="33" t="s">
+        <v>396</v>
+      </c>
+      <c r="B50" s="57" t="s">
+        <v>394</v>
+      </c>
+      <c r="D50" s="43" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A51" s="33" t="s">
+        <v>396</v>
+      </c>
+      <c r="B51" s="57" t="s">
+        <v>395</v>
+      </c>
+      <c r="D51" s="43" t="s">
+        <v>334</v>
       </c>
     </row>
   </sheetData>

</xml_diff>